<commit_message>
partial completion of live stuff. Updated documentation from stand up on Nov 30.
</commit_message>
<xml_diff>
--- a/docs/Sprint 2/Sprint2Burndown.xlsx
+++ b/docs/Sprint 2/Sprint2Burndown.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexm\Box\Fall19\Repo-1.01\docs\plannning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexm\Box\Fall19\Repo-1.01\docs\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A8A293-352B-4E09-B439-6019DC4A7B12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA74B1B-D331-49E1-ACC3-1F8FA8EDD188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,8 +128,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Burndown Chart  for Sprint 2 as of October 28</a:t>
+              <a:t>Burndown Chart  for Sprint 2 as of</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> November 4</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -267,13 +272,13 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -700,7 +705,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -749,7 +754,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -760,7 +765,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -771,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs for end of sprint 2
</commit_message>
<xml_diff>
--- a/docs/Sprint 2/Sprint2Burndown.xlsx
+++ b/docs/Sprint 2/Sprint2Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexm\Box\Fall19\Repo-1.01\docs\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA74B1B-D331-49E1-ACC3-1F8FA8EDD188}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1BA6CB-A9C8-4EE0-945B-6A3AB8B1F9DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,7 +132,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> November 4</a:t>
+              <a:t> November 8</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -278,7 +278,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -705,7 +705,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -776,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>